<commit_message>
minor update to xp chart
</commit_message>
<xml_diff>
--- a/00XPChart.xlsx
+++ b/00XPChart.xlsx
@@ -178,7 +178,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,8 +221,8 @@
   </sheetPr>
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -249,7 +249,7 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -403,35 +403,35 @@
       </c>
       <c r="G12" s="6" t="n">
         <f aca="false">J12*(1-(3*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="H12" s="6" t="n">
         <f aca="false">J12*(1-(2*$D$10))</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="I12" s="6" t="n">
         <f aca="false">J12*(1-$D$10)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="J12" s="6" t="n">
-        <f aca="false">C12/D12</f>
-        <v>25</v>
+        <f aca="false">C12/D12*$D$1</f>
+        <v>75</v>
       </c>
       <c r="K12" s="6" t="n">
         <f aca="false">J12*(1+$D$9)</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="L12" s="6" t="n">
         <f aca="false">J12*(1+($D$9*2))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="M12" s="6" t="n">
         <f aca="false">J12*((1+4*$D$9))</f>
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="N12" s="6" t="n">
         <f aca="false">J12*((1+6*$D$9))</f>
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,35 +460,35 @@
       </c>
       <c r="G13" s="6" t="n">
         <f aca="false">J13*(1-(3*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="H13" s="6" t="n">
         <f aca="false">J13*(1-(2*$D$10))</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="I13" s="6" t="n">
         <f aca="false">J13*(1-$D$10)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="J13" s="6" t="n">
-        <f aca="false">C13/D13</f>
-        <v>25</v>
+        <f aca="false">C13/D13*$D$1</f>
+        <v>75</v>
       </c>
       <c r="K13" s="6" t="n">
         <f aca="false">J13*(1+$D$9)</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="L13" s="6" t="n">
         <f aca="false">J13*(1+($D$9*2))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="M13" s="6" t="n">
         <f aca="false">J13*((1+4*$D$9))</f>
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="N13" s="6" t="n">
         <f aca="false">J13*((1+6*$D$9))</f>
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,35 +517,35 @@
       </c>
       <c r="G14" s="6" t="n">
         <f aca="false">J14*(1-(3*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="H14" s="6" t="n">
         <f aca="false">J14*(1-(2*$D$10))</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="I14" s="6" t="n">
         <f aca="false">J14*(1-$D$10)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="J14" s="6" t="n">
-        <f aca="false">C14/D14</f>
-        <v>25</v>
+        <f aca="false">C14/D14*$D$1</f>
+        <v>75</v>
       </c>
       <c r="K14" s="6" t="n">
         <f aca="false">J14*(1+$D$9)</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="L14" s="6" t="n">
         <f aca="false">J14*(1+($D$9*2))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="M14" s="6" t="n">
         <f aca="false">J14*((1+4*$D$9))</f>
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="N14" s="6" t="n">
         <f aca="false">J14*((1+6*$D$9))</f>
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,35 +574,35 @@
       </c>
       <c r="G15" s="6" t="n">
         <f aca="false">J15*(1-(3*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="H15" s="6" t="n">
         <f aca="false">J15*(1-(2*$D$10))</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="I15" s="6" t="n">
         <f aca="false">J15*(1-$D$10)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="J15" s="6" t="n">
-        <f aca="false">C15/D15</f>
-        <v>25</v>
+        <f aca="false">C15/D15*$D$1</f>
+        <v>75</v>
       </c>
       <c r="K15" s="6" t="n">
         <f aca="false">J15*(1+$D$9)</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="L15" s="6" t="n">
         <f aca="false">J15*(1+($D$9*2))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="M15" s="6" t="n">
         <f aca="false">J15*((1+4*$D$9))</f>
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="N15" s="6" t="n">
         <f aca="false">J15*((1+6*$D$9))</f>
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,35 +631,35 @@
       </c>
       <c r="G16" s="6" t="n">
         <f aca="false">J16*(1-(3*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="H16" s="6" t="n">
         <f aca="false">J16*(1-(2*$D$10))</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="I16" s="6" t="n">
         <f aca="false">J16*(1-$D$10)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="J16" s="6" t="n">
-        <f aca="false">C16/D16</f>
-        <v>25</v>
+        <f aca="false">C16/D16*$D$1</f>
+        <v>75</v>
       </c>
       <c r="K16" s="6" t="n">
         <f aca="false">J16*(1+$D$9)</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="L16" s="6" t="n">
         <f aca="false">J16*(1+($D$9*2))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="M16" s="6" t="n">
         <f aca="false">J16*((1+4*$D$9))</f>
-        <v>75</v>
+        <v>225</v>
       </c>
       <c r="N16" s="6" t="n">
         <f aca="false">J16*((1+6*$D$9))</f>
-        <v>100</v>
+        <v>300</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -688,35 +688,35 @@
       </c>
       <c r="G17" s="6" t="n">
         <f aca="false">J17*(1-(3*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="H17" s="6" t="n">
         <f aca="false">J17*(1-(2*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="I17" s="6" t="n">
         <f aca="false">J17*(1-$D$10)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="J17" s="6" t="n">
-        <f aca="false">C17/D17</f>
-        <v>12.5</v>
+        <f aca="false">C17/D17*$D$1</f>
+        <v>37.5</v>
       </c>
       <c r="K17" s="6" t="n">
         <f aca="false">J17*(1+$D$9)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="L17" s="6" t="n">
         <f aca="false">J17*(1+($D$9*2))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M17" s="6" t="n">
         <f aca="false">J17*((1+4*$D$9))</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="N17" s="6" t="n">
         <f aca="false">J17*((1+6*$D$9))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,35 +745,35 @@
       </c>
       <c r="G18" s="6" t="n">
         <f aca="false">J18*(1-(3*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="H18" s="6" t="n">
         <f aca="false">J18*(1-(2*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="I18" s="6" t="n">
         <f aca="false">J18*(1-$D$10)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="J18" s="6" t="n">
-        <f aca="false">C18/D18</f>
-        <v>12.5</v>
+        <f aca="false">C18/D18*$D$1</f>
+        <v>37.5</v>
       </c>
       <c r="K18" s="6" t="n">
         <f aca="false">J18*(1+$D$9)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="L18" s="6" t="n">
         <f aca="false">J18*(1+($D$9*2))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M18" s="6" t="n">
         <f aca="false">J18*((1+4*$D$9))</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="N18" s="6" t="n">
         <f aca="false">J18*((1+6*$D$9))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,35 +802,35 @@
       </c>
       <c r="G19" s="6" t="n">
         <f aca="false">J19*(1-(3*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="H19" s="6" t="n">
         <f aca="false">J19*(1-(2*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="I19" s="6" t="n">
         <f aca="false">J19*(1-$D$10)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="J19" s="6" t="n">
-        <f aca="false">C19/D19</f>
-        <v>12.5</v>
+        <f aca="false">C19/D19*$D$1</f>
+        <v>37.5</v>
       </c>
       <c r="K19" s="6" t="n">
         <f aca="false">J19*(1+$D$9)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="L19" s="6" t="n">
         <f aca="false">J19*(1+($D$9*2))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M19" s="6" t="n">
         <f aca="false">J19*((1+4*$D$9))</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="N19" s="6" t="n">
         <f aca="false">J19*((1+6*$D$9))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,35 +859,35 @@
       </c>
       <c r="G20" s="6" t="n">
         <f aca="false">J20*(1-(3*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="H20" s="6" t="n">
         <f aca="false">J20*(1-(2*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="I20" s="6" t="n">
         <f aca="false">J20*(1-$D$10)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="J20" s="6" t="n">
-        <f aca="false">C20/D20</f>
-        <v>12.5</v>
+        <f aca="false">C20/D20*$D$1</f>
+        <v>37.5</v>
       </c>
       <c r="K20" s="6" t="n">
         <f aca="false">J20*(1+$D$9)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="L20" s="6" t="n">
         <f aca="false">J20*(1+($D$9*2))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M20" s="6" t="n">
         <f aca="false">J20*((1+4*$D$9))</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="N20" s="6" t="n">
         <f aca="false">J20*((1+6*$D$9))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,35 +916,35 @@
       </c>
       <c r="G21" s="6" t="n">
         <f aca="false">J21*(1-(3*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="H21" s="6" t="n">
         <f aca="false">J21*(1-(2*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="I21" s="6" t="n">
         <f aca="false">J21*(1-$D$10)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="J21" s="6" t="n">
-        <f aca="false">C21/D21</f>
-        <v>12.5</v>
+        <f aca="false">C21/D21*$D$1</f>
+        <v>37.5</v>
       </c>
       <c r="K21" s="6" t="n">
         <f aca="false">J21*(1+$D$9)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="L21" s="6" t="n">
         <f aca="false">J21*(1+($D$9*2))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M21" s="6" t="n">
         <f aca="false">J21*((1+4*$D$9))</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="N21" s="6" t="n">
         <f aca="false">J21*((1+6*$D$9))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,35 +973,35 @@
       </c>
       <c r="G22" s="6" t="n">
         <f aca="false">J22*(1-(3*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="H22" s="6" t="n">
         <f aca="false">J22*(1-(2*$D$10))</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="I22" s="6" t="n">
         <f aca="false">J22*(1-$D$10)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="J22" s="6" t="n">
-        <f aca="false">C22/D22</f>
-        <v>12.5</v>
+        <f aca="false">C22/D22*$D$1</f>
+        <v>37.5</v>
       </c>
       <c r="K22" s="6" t="n">
         <f aca="false">J22*(1+$D$9)</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="L22" s="6" t="n">
         <f aca="false">J22*(1+($D$9*2))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="M22" s="6" t="n">
         <f aca="false">J22*((1+4*$D$9))</f>
-        <v>37.5</v>
+        <v>112.5</v>
       </c>
       <c r="N22" s="6" t="n">
         <f aca="false">J22*((1+6*$D$9))</f>
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1030,35 +1030,35 @@
       </c>
       <c r="G23" s="6" t="n">
         <f aca="false">J23*(1-(3*$D$10))</f>
-        <v>2.08333333333333</v>
+        <v>6.25</v>
       </c>
       <c r="H23" s="6" t="n">
         <f aca="false">J23*(1-(2*$D$10))</f>
-        <v>4.16666666666667</v>
+        <v>12.5</v>
       </c>
       <c r="I23" s="6" t="n">
         <f aca="false">J23*(1-$D$10)</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="J23" s="6" t="n">
-        <f aca="false">C23/D23</f>
-        <v>8.33333333333333</v>
+        <f aca="false">C23/D23*$D$1</f>
+        <v>25</v>
       </c>
       <c r="K23" s="6" t="n">
         <f aca="false">J23*(1+$D$9)</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="L23" s="6" t="n">
         <f aca="false">J23*(1+($D$9*2))</f>
-        <v>16.6666666666667</v>
+        <v>50</v>
       </c>
       <c r="M23" s="6" t="n">
         <f aca="false">J23*((1+4*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N23" s="6" t="n">
         <f aca="false">J23*((1+6*$D$9))</f>
-        <v>33.3333333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1087,35 +1087,35 @@
       </c>
       <c r="G24" s="6" t="n">
         <f aca="false">J24*(1-(3*$D$10))</f>
-        <v>2.08333333333333</v>
+        <v>6.25</v>
       </c>
       <c r="H24" s="6" t="n">
         <f aca="false">J24*(1-(2*$D$10))</f>
-        <v>4.16666666666667</v>
+        <v>12.5</v>
       </c>
       <c r="I24" s="6" t="n">
         <f aca="false">J24*(1-$D$10)</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="J24" s="6" t="n">
-        <f aca="false">C24/D24</f>
-        <v>8.33333333333333</v>
+        <f aca="false">C24/D24*$D$1</f>
+        <v>25</v>
       </c>
       <c r="K24" s="6" t="n">
         <f aca="false">J24*(1+$D$9)</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="L24" s="6" t="n">
         <f aca="false">J24*(1+($D$9*2))</f>
-        <v>16.6666666666667</v>
+        <v>50</v>
       </c>
       <c r="M24" s="6" t="n">
         <f aca="false">J24*((1+4*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N24" s="6" t="n">
         <f aca="false">J24*((1+6*$D$9))</f>
-        <v>33.3333333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,35 +1144,35 @@
       </c>
       <c r="G25" s="6" t="n">
         <f aca="false">J25*(1-(3*$D$10))</f>
-        <v>2.08333333333333</v>
+        <v>6.25</v>
       </c>
       <c r="H25" s="6" t="n">
         <f aca="false">J25*(1-(2*$D$10))</f>
-        <v>4.16666666666667</v>
+        <v>12.5</v>
       </c>
       <c r="I25" s="6" t="n">
         <f aca="false">J25*(1-$D$10)</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="J25" s="6" t="n">
-        <f aca="false">C25/D25</f>
-        <v>8.33333333333333</v>
+        <f aca="false">C25/D25*$D$1</f>
+        <v>25</v>
       </c>
       <c r="K25" s="6" t="n">
         <f aca="false">J25*(1+$D$9)</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="L25" s="6" t="n">
         <f aca="false">J25*(1+($D$9*2))</f>
-        <v>16.6666666666667</v>
+        <v>50</v>
       </c>
       <c r="M25" s="6" t="n">
         <f aca="false">J25*((1+4*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N25" s="6" t="n">
         <f aca="false">J25*((1+6*$D$9))</f>
-        <v>33.3333333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,35 +1201,35 @@
       </c>
       <c r="G26" s="6" t="n">
         <f aca="false">J26*(1-(3*$D$10))</f>
-        <v>2.08333333333333</v>
+        <v>6.25</v>
       </c>
       <c r="H26" s="6" t="n">
         <f aca="false">J26*(1-(2*$D$10))</f>
-        <v>4.16666666666667</v>
+        <v>12.5</v>
       </c>
       <c r="I26" s="6" t="n">
         <f aca="false">J26*(1-$D$10)</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="J26" s="6" t="n">
-        <f aca="false">C26/D26</f>
-        <v>8.33333333333333</v>
+        <f aca="false">C26/D26*$D$1</f>
+        <v>25</v>
       </c>
       <c r="K26" s="6" t="n">
         <f aca="false">J26*(1+$D$9)</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="L26" s="6" t="n">
         <f aca="false">J26*(1+($D$9*2))</f>
-        <v>16.6666666666667</v>
+        <v>50</v>
       </c>
       <c r="M26" s="6" t="n">
         <f aca="false">J26*((1+4*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N26" s="6" t="n">
         <f aca="false">J26*((1+6*$D$9))</f>
-        <v>33.3333333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,35 +1258,35 @@
       </c>
       <c r="G27" s="6" t="n">
         <f aca="false">J27*(1-(3*$D$10))</f>
-        <v>2.08333333333333</v>
+        <v>6.25</v>
       </c>
       <c r="H27" s="6" t="n">
         <f aca="false">J27*(1-(2*$D$10))</f>
-        <v>4.16666666666667</v>
+        <v>12.5</v>
       </c>
       <c r="I27" s="6" t="n">
         <f aca="false">J27*(1-$D$10)</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="J27" s="6" t="n">
-        <f aca="false">C27/D27</f>
-        <v>8.33333333333333</v>
+        <f aca="false">C27/D27*$D$1</f>
+        <v>25</v>
       </c>
       <c r="K27" s="6" t="n">
         <f aca="false">J27*(1+$D$9)</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="L27" s="6" t="n">
         <f aca="false">J27*(1+($D$9*2))</f>
-        <v>16.6666666666667</v>
+        <v>50</v>
       </c>
       <c r="M27" s="6" t="n">
         <f aca="false">J27*((1+4*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N27" s="6" t="n">
         <f aca="false">J27*((1+6*$D$9))</f>
-        <v>33.3333333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1315,35 +1315,35 @@
       </c>
       <c r="G28" s="6" t="n">
         <f aca="false">J28*(1-(3*$D$10))</f>
-        <v>2.08333333333333</v>
+        <v>6.25</v>
       </c>
       <c r="H28" s="6" t="n">
         <f aca="false">J28*(1-(2*$D$10))</f>
-        <v>4.16666666666667</v>
+        <v>12.5</v>
       </c>
       <c r="I28" s="6" t="n">
         <f aca="false">J28*(1-$D$10)</f>
-        <v>6.25</v>
+        <v>18.75</v>
       </c>
       <c r="J28" s="6" t="n">
-        <f aca="false">C28/D28</f>
-        <v>8.33333333333333</v>
+        <f aca="false">C28/D28*$D$1</f>
+        <v>25</v>
       </c>
       <c r="K28" s="6" t="n">
         <f aca="false">J28*(1+$D$9)</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="L28" s="6" t="n">
         <f aca="false">J28*(1+($D$9*2))</f>
-        <v>16.6666666666667</v>
+        <v>50</v>
       </c>
       <c r="M28" s="6" t="n">
         <f aca="false">J28*((1+4*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="N28" s="6" t="n">
         <f aca="false">J28*((1+6*$D$9))</f>
-        <v>33.3333333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,35 +1372,35 @@
       </c>
       <c r="G29" s="6" t="n">
         <f aca="false">J29*(1-(3*$D$10))</f>
-        <v>1.5625</v>
+        <v>4.6875</v>
       </c>
       <c r="H29" s="6" t="n">
         <f aca="false">J29*(1-(2*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="I29" s="6" t="n">
         <f aca="false">J29*(1-$D$10)</f>
-        <v>4.6875</v>
+        <v>14.0625</v>
       </c>
       <c r="J29" s="6" t="n">
-        <f aca="false">C29/D29</f>
-        <v>6.25</v>
+        <f aca="false">C29/D29*$D$1</f>
+        <v>18.75</v>
       </c>
       <c r="K29" s="6" t="n">
         <f aca="false">J29*(1+$D$9)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="L29" s="6" t="n">
         <f aca="false">J29*(1+($D$9*2))</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="M29" s="6" t="n">
         <f aca="false">J29*((1+4*$D$9))</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="N29" s="6" t="n">
         <f aca="false">J29*((1+6*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1429,35 +1429,35 @@
       </c>
       <c r="G30" s="6" t="n">
         <f aca="false">J30*(1-(3*$D$10))</f>
-        <v>1.5625</v>
+        <v>4.6875</v>
       </c>
       <c r="H30" s="6" t="n">
         <f aca="false">J30*(1-(2*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="I30" s="6" t="n">
         <f aca="false">J30*(1-$D$10)</f>
-        <v>4.6875</v>
+        <v>14.0625</v>
       </c>
       <c r="J30" s="6" t="n">
-        <f aca="false">C30/D30</f>
-        <v>6.25</v>
+        <f aca="false">C30/D30*$D$1</f>
+        <v>18.75</v>
       </c>
       <c r="K30" s="6" t="n">
         <f aca="false">J30*(1+$D$9)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="L30" s="6" t="n">
         <f aca="false">J30*(1+($D$9*2))</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="M30" s="6" t="n">
         <f aca="false">J30*((1+4*$D$9))</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="N30" s="6" t="n">
         <f aca="false">J30*((1+6*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,35 +1486,35 @@
       </c>
       <c r="G31" s="6" t="n">
         <f aca="false">J31*(1-(3*$D$10))</f>
-        <v>1.5625</v>
+        <v>4.6875</v>
       </c>
       <c r="H31" s="6" t="n">
         <f aca="false">J31*(1-(2*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="I31" s="6" t="n">
         <f aca="false">J31*(1-$D$10)</f>
-        <v>4.6875</v>
+        <v>14.0625</v>
       </c>
       <c r="J31" s="6" t="n">
-        <f aca="false">C31/D31</f>
-        <v>6.25</v>
+        <f aca="false">C31/D31*$D$1</f>
+        <v>18.75</v>
       </c>
       <c r="K31" s="6" t="n">
         <f aca="false">J31*(1+$D$9)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="L31" s="6" t="n">
         <f aca="false">J31*(1+($D$9*2))</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="M31" s="6" t="n">
         <f aca="false">J31*((1+4*$D$9))</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="N31" s="6" t="n">
         <f aca="false">J31*((1+6*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,35 +1542,35 @@
       </c>
       <c r="G32" s="6" t="n">
         <f aca="false">J32*(1-(3*$D$10))</f>
-        <v>1.5625</v>
+        <v>4.6875</v>
       </c>
       <c r="H32" s="6" t="n">
         <f aca="false">J32*(1-(2*$D$10))</f>
-        <v>3.125</v>
+        <v>9.375</v>
       </c>
       <c r="I32" s="6" t="n">
         <f aca="false">J32*(1-$D$10)</f>
-        <v>4.6875</v>
+        <v>14.0625</v>
       </c>
       <c r="J32" s="6" t="n">
-        <f aca="false">C32/D32</f>
-        <v>6.25</v>
+        <f aca="false">C32/D32*$D$1</f>
+        <v>18.75</v>
       </c>
       <c r="K32" s="6" t="n">
         <f aca="false">J32*(1+$D$9)</f>
-        <v>9.375</v>
+        <v>28.125</v>
       </c>
       <c r="L32" s="6" t="n">
         <f aca="false">J32*(1+($D$9*2))</f>
-        <v>12.5</v>
+        <v>37.5</v>
       </c>
       <c r="M32" s="6" t="n">
         <f aca="false">J32*((1+4*$D$9))</f>
-        <v>18.75</v>
+        <v>56.25</v>
       </c>
       <c r="N32" s="6" t="n">
         <f aca="false">J32*((1+6*$D$9))</f>
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>